<commit_message>
DEV2.1 - Application Management
</commit_message>
<xml_diff>
--- a/resources/data/ProjectApplication.xlsx
+++ b/resources/data/ProjectApplication.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a02774ed8d28bca/Desktop/NTU/NTU_Y1S2/SC2002/Assignment/BTO_Application/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/racshanyaa/Documents/GitHub/SC2002-BTO-V3/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42CCDBA0-F3FB-42E1-BBBA-0B020E9235B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62902B0-8BB2-6245-BB69-39C62CCD9BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="1103" windowWidth="13050" windowHeight="11767" xr2:uid="{0D642D4F-2CEA-46CE-BAFD-529E47B214DF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19240" xr2:uid="{0D642D4F-2CEA-46CE-BAFD-529E47B214DF}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectApplication" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,50 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+  <si>
+    <t>Application ID</t>
+  </si>
+  <si>
+    <t>Applicant NRIC</t>
+  </si>
+  <si>
+    <t>Application Status</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Project ID</t>
+  </si>
+  <si>
+    <t>S1234567A</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Thu Apr 17 18:46:06 SGT 2025</t>
+  </si>
+  <si>
+    <t>Thu Apr 17 18:46:29 SGT 2025</t>
+  </si>
+  <si>
+    <t>Withdrawn</t>
+  </si>
+  <si>
+    <t>Thu Apr 17 18:46:41 SGT 2025</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -498,8 +540,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -875,12 +918,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990A7129-9B77-400F-B045-4AF64172596B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="A4" sqref="A3:E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.5" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished Application and touched up a few manager views
Manager views need to have input validation for integers (NOT DONE)

Manager needs to streamline options to have less words and more options eg. 1 2 3 4 options (NOT DONE)

Manager applications should filter by "withdrawal pending" and "pending" status instead of listing everything to the manager (NOT DONE)
</commit_message>
<xml_diff>
--- a/resources/data/ProjectApplication.xlsx
+++ b/resources/data/ProjectApplication.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/racshanyaa/Documents/GitHub/SC2002-BTO-V3/resources/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a02774ed8d28bca/Documents/GitHub/SC2002-BTO-V3/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62902B0-8BB2-6245-BB69-39C62CCD9BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{A62902B0-8BB2-6245-BB69-39C62CCD9BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3054B518-92C5-498C-A23F-C8CE800F69A5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19240" xr2:uid="{0D642D4F-2CEA-46CE-BAFD-529E47B214DF}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{0D642D4F-2CEA-46CE-BAFD-529E47B214DF}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectApplication" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Application ID</t>
   </si>
@@ -31,31 +31,31 @@
     <t>Application Status</t>
   </si>
   <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Project ID</t>
+  </si>
+  <si>
+    <t>Flat Type</t>
+  </si>
+  <si>
+    <t>S1234567A</t>
+  </si>
+  <si>
     <t>Pending</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Project ID</t>
-  </si>
-  <si>
-    <t>S1234567A</t>
-  </si>
-  <si>
-    <t>Success</t>
-  </si>
-  <si>
-    <t>Thu Apr 17 18:46:06 SGT 2025</t>
-  </si>
-  <si>
-    <t>Thu Apr 17 18:46:29 SGT 2025</t>
-  </si>
-  <si>
-    <t>Withdrawn</t>
-  </si>
-  <si>
-    <t>Thu Apr 17 18:46:41 SGT 2025</t>
+    <t>2-ROOM</t>
+  </si>
+  <si>
+    <t>Successful</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Withdrawal Pending</t>
   </si>
 </sst>
 </file>
@@ -542,7 +542,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -599,6 +599,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -918,26 +922,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990A7129-9B77-400F-B045-4AF64172596B}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="A4" sqref="A3:E4"/>
+    <sheetView tabSelected="1" topLeftCell="A1048559" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A1048576" sqref="A3:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="11.46484375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="11.0" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.5" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.46484375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -946,24 +950,30 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" t="n">
+        <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="n">
+        <v>45767.18201704861</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Abit of officer stuff
</commit_message>
<xml_diff>
--- a/resources/data/ProjectApplication.xlsx
+++ b/resources/data/ProjectApplication.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a02774ed8d28bca/Documents/GitHub/SC2002-BTO-V3/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{A62902B0-8BB2-6245-BB69-39C62CCD9BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3054B518-92C5-498C-A23F-C8CE800F69A5}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{A62902B0-8BB2-6245-BB69-39C62CCD9BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{111D456F-3969-4B2D-B6B6-ED43018F4088}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{0D642D4F-2CEA-46CE-BAFD-529E47B214DF}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Application ID</t>
   </si>
@@ -39,30 +39,11 @@
   <si>
     <t>Flat Type</t>
   </si>
-  <si>
-    <t>S1234567A</t>
-  </si>
-  <si>
-    <t>Pending</t>
-  </si>
-  <si>
-    <t>2-ROOM</t>
-  </si>
-  <si>
-    <t>Successful</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>Withdrawal Pending</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -922,18 +903,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990A7129-9B77-400F-B045-4AF64172596B}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1048559" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A1048576" sqref="A3:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="11.46484375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="11.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.46484375" collapsed="true"/>
+    <col min="1" max="1" width="11.46484375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.46484375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -956,26 +937,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="n">
-        <v>45767.18201704861</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
DEV 12 - Project Global Deletion
</commit_message>
<xml_diff>
--- a/resources/data/ProjectApplication.xlsx
+++ b/resources/data/ProjectApplication.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/racshanyaa/Documents/GitHub/SC2002-BTO-V3/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2E04A7-185E-8A4A-A300-B1679E2FF9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB980AD0-B36C-3546-8DAD-989C46FC7922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="1020" windowWidth="14580" windowHeight="11760" xr2:uid="{0D642D4F-2CEA-46CE-BAFD-529E47B214DF}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Application ID</t>
   </si>
@@ -58,7 +58,10 @@
     <t>T2345678D</t>
   </si>
   <si>
-    <t>Successful</t>
+    <t>T7654321B</t>
+  </si>
+  <si>
+    <t>Deleted</t>
   </si>
 </sst>
 </file>
@@ -921,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990A7129-9B77-400F-B045-4AF64172596B}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -956,23 +959,23 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
+      <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2.0</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2">
-        <v>45769.835042048609</v>
+      <c r="F2" t="n">
+        <v>45771.12818586805</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -986,13 +989,13 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
       <c r="F3" t="n">
-        <v>45770.468184178244</v>
+        <v>45771.128186712966</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1012,6 +1015,26 @@
         <v>8</v>
       </c>
       <c r="F4">
+        <v>45769.900285069445</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5">
         <v>45769.900285069445</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DEV 13 - Bug Fix and MVC Project, Application, Enquiry
</commit_message>
<xml_diff>
--- a/resources/data/ProjectApplication.xlsx
+++ b/resources/data/ProjectApplication.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/racshanyaa/Documents/GitHub/SC2002-BTO-V3/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB980AD0-B36C-3546-8DAD-989C46FC7922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D1C0EA-DF94-EA4B-BE5D-700BBF667D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="1020" windowWidth="14580" windowHeight="11760" xr2:uid="{0D642D4F-2CEA-46CE-BAFD-529E47B214DF}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Application ID</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>S1234567A</t>
-  </si>
-  <si>
-    <t>Withdrawal Pending</t>
   </si>
   <si>
     <t>T2345678D</t>
@@ -68,7 +65,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -927,15 +923,15 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:F5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="11.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="11.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.5" collapsed="true"/>
+    <col min="1" max="1" width="11.5" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -959,42 +955,42 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>2.0</v>
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="n">
-        <v>45771.12818586805</v>
+      <c r="F2">
+        <v>45771.128185868052</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2.0</v>
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>45771.128186712966</v>
       </c>
     </row>
@@ -1006,7 +1002,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1026,7 +1022,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>

</xml_diff>